<commit_message>
One more progress fix
</commit_message>
<xml_diff>
--- a/TestRelated/Tests.xlsx
+++ b/TestRelated/Tests.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\WorldConstructor\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\FileBackup\TestRelated\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D396B54-E02B-4C0F-8397-65C0A93A26BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CF7B625-CC2E-4D41-9BAF-1D4B5357CF25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="21000" yWindow="6525" windowWidth="22410" windowHeight="15345" activeTab="1" xr2:uid="{7E419EB6-8C87-46B1-89F4-388E9138BF20}"/>
+    <workbookView xWindow="9390" yWindow="0" windowWidth="19515" windowHeight="15585" xr2:uid="{7E419EB6-8C87-46B1-89F4-388E9138BF20}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="45">
   <si>
     <t>Change</t>
   </si>
@@ -134,6 +134,41 @@
   </si>
   <si>
     <t>Files that exceed the file limit when checked against moving them</t>
+  </si>
+  <si>
+    <t>No change</t>
+  </si>
+  <si>
+    <t>Speciific test</t>
+  </si>
+  <si>
+    <t>Multiple files / directories</t>
+  </si>
+  <si>
+    <t>Passed?</t>
+  </si>
+  <si>
+    <t>Verify full copy
+Verify duplicate report (if applicable)
+Verify copy list</t>
+  </si>
+  <si>
+    <t>Removed duplicate files, only delete report was created, as files were not archived (since they already existed)</t>
+  </si>
+  <si>
+    <t>Removed files that were not duplicates, saw generated archive with files that were removed.</t>
+  </si>
+  <si>
+    <t>Removed all files, including duplicate groups.  Saw generated archive with files that were removed including duplicates.  Note ideal, but okay.</t>
+  </si>
+  <si>
+    <t>Renamed 3 documents</t>
+  </si>
+  <si>
+    <t>Renamed single file</t>
+  </si>
+  <si>
+    <t>Single files, no dirs</t>
   </si>
 </sst>
 </file>
@@ -169,10 +204,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -488,67 +527,154 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C108830-0206-42B8-BBF8-8D72AD8B6130}">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="26" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="60.140625" customWidth="1"/>
+    <col min="2" max="2" width="60.140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="24.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+      <c r="C1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D2" s="2">
+        <v>45564</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="3"/>
+      <c r="B3" s="3"/>
+      <c r="C3" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D3" s="2">
+        <v>45564</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B4" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+      <c r="C4" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D4" s="2">
+        <v>45564</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C5" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D5" s="2">
+        <v>45564</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B6" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+      <c r="D6" s="2">
+        <v>45564</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B7" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
+      <c r="C7" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D7" s="2">
+        <v>45564</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="B8" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D8" s="2">
+        <v>45564</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="105" x14ac:dyDescent="0.25">
+      <c r="B9" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D9" s="2">
+        <v>45564</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B10" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
+      <c r="D10" s="2">
+        <v>45564</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B11" s="1" t="s">
         <v>11</v>
       </c>
+      <c r="D11" s="2">
+        <v>45564</v>
+      </c>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="B2:B3"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -557,7 +683,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8141AC55-CB84-4A57-B433-0EE1EDE0DD86}">
   <dimension ref="A1:B25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>

</xml_diff>